<commit_message>
WRI edits to files where EI identified issues
</commit_message>
<xml_diff>
--- a/InputData/fuels/BSoFPtiT/BAU Share of Fuel Price that is Tax.xlsx
+++ b/InputData/fuels/BSoFPtiT/BAU Share of Fuel Price that is Tax.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23258" windowHeight="12578"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11505"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2332,7 +2332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -29800,7 +29800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -30626,6 +30628,20 @@
         <f>E8/E9</f>
         <v>1.4633182249393908E-2</v>
       </c>
+    </row>
+    <row r="11" spans="1:80" x14ac:dyDescent="0.45">
+      <c r="D11" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1.4633182249393908E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:80" x14ac:dyDescent="0.45">
+      <c r="D12" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="E12" s="17"/>
     </row>
     <row r="16" spans="1:80" x14ac:dyDescent="0.45">
       <c r="B16" s="59"/>
@@ -33223,10 +33239,10 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AK27"/>
+  <dimension ref="A1:AK22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -33236,436 +33252,1057 @@
     <col min="3" max="3" width="8.796875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
-        <v>375</v>
-      </c>
-      <c r="B1" s="17">
-        <v>1.4633182249393908E-2</v>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="18">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="18">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2028</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2029</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2035</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2036</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2037</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2038</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>2039</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>2040</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>2041</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>2042</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>2043</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>2044</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>2045</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>2047</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>2049</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="17" t="s">
-        <v>376</v>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="C2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="D2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="E2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="F2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="G2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="H2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="I2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="J2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="K2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="L2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="M2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="N2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="O2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="P2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Q2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="R2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="S2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="T2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="U2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="V2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="W2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="X2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Y2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Z2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AA2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AB2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AC2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AD2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AE2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AF2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AG2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AH2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AI2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AJ2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AK2" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="C3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="D3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="E3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="F3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="G3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="H3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="I3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="J3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="K3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="L3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="M3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="N3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="O3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="P3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Q3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="R3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="S3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="T3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="U3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="V3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="W3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="X3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Y3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Z3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AA3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AB3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AC3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AD3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AE3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AF3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AG3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AH3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AI3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AJ3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AK3" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="C4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="D4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="E4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="F4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="G4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="H4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="I4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="J4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="K4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="L4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="M4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="N4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="O4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="P4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Q4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="R4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="S4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="T4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="U4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="V4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="W4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="X4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Y4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Z4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AA4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AB4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AC4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AD4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AE4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AF4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AG4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AH4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AI4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AJ4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AK4" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="C5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="D5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="E5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="F5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="G5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="H5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="I5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="J5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="K5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="L5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="M5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="N5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="O5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="P5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Q5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="R5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="S5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="T5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="U5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="V5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="W5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="X5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Y5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Z5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AA5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AB5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AC5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AD5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AE5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AF5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AG5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AH5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AI5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AJ5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AK5" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+    </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="18">
-        <v>2015</v>
-      </c>
-      <c r="C6" s="18">
-        <v>2016</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G6" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H6" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I6" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J6" s="1">
-        <v>2023</v>
-      </c>
-      <c r="K6" s="1">
-        <v>2024</v>
-      </c>
-      <c r="L6" s="1">
-        <v>2025</v>
-      </c>
-      <c r="M6" s="1">
-        <v>2026</v>
-      </c>
-      <c r="N6" s="1">
-        <v>2027</v>
-      </c>
-      <c r="O6" s="1">
-        <v>2028</v>
-      </c>
-      <c r="P6" s="1">
-        <v>2029</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>2030</v>
-      </c>
-      <c r="R6" s="1">
-        <v>2031</v>
-      </c>
-      <c r="S6" s="1">
-        <v>2032</v>
-      </c>
-      <c r="T6" s="1">
-        <v>2033</v>
-      </c>
-      <c r="U6" s="1">
-        <v>2034</v>
-      </c>
-      <c r="V6" s="1">
-        <v>2035</v>
-      </c>
-      <c r="W6" s="1">
-        <v>2036</v>
-      </c>
-      <c r="X6" s="1">
-        <v>2037</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>2038</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>2039</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>2040</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>2041</v>
-      </c>
-      <c r="AC6" s="1">
-        <v>2042</v>
-      </c>
-      <c r="AD6" s="1">
-        <v>2043</v>
-      </c>
-      <c r="AE6" s="1">
-        <v>2044</v>
-      </c>
-      <c r="AF6" s="1">
-        <v>2045</v>
-      </c>
-      <c r="AG6" s="1">
-        <v>2046</v>
-      </c>
-      <c r="AH6" s="1">
-        <v>2047</v>
-      </c>
-      <c r="AI6" s="1">
-        <v>2048</v>
-      </c>
-      <c r="AJ6" s="1">
-        <v>2049</v>
-      </c>
-      <c r="AK6" s="1">
-        <v>2050</v>
+        <v>8</v>
+      </c>
+      <c r="B6" s="17">
+        <v>0</v>
+      </c>
+      <c r="C6" s="17">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="C7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="D7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="E7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="F7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="G7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="H7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="I7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="J7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="K7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="L7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="M7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="N7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="O7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="P7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Q7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="R7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="S7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="T7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="U7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="V7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="W7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="X7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Y7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Z7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AA7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AB7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AC7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AD7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AE7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AF7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AG7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AH7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AI7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AJ7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AK7" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
+        <v>9</v>
+      </c>
+      <c r="B7" s="17">
+        <v>0</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="C8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="D8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="E8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="F8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="G8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="H8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="I8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="J8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="K8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="L8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="M8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="N8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="O8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="P8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Q8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="R8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="S8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="T8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="U8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="V8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="W8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="X8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Y8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Z8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AA8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AB8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AC8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AD8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AE8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AF8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AG8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AH8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AI8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AJ8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AK8" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
+        <v>20</v>
+      </c>
+      <c r="B8" s="17">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B9" s="49">
         <f>About!$C$33</f>
@@ -33813,496 +34450,604 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="C10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="D10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="E10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="F10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="G10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="H10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="I10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="J10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="K10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="L10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="M10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="N10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="O10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="P10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Q10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="R10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="S10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="T10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="U10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="V10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="W10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="X10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Y10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Z10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AA10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AB10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AC10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AD10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AE10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AF10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AG10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AH10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AI10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AJ10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AK10" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
+      <c r="A10" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="20">
+        <f>E10</f>
+        <v>0.43497623825544579</v>
+      </c>
+      <c r="C10" s="20">
+        <f>E10</f>
+        <v>0.43497623825544579</v>
+      </c>
+      <c r="D10" s="4">
+        <f>E10</f>
+        <v>0.43497623825544579</v>
+      </c>
+      <c r="E10" s="20">
+        <f>SUM(INDEX(Petroleum!$C$21:$E$22,0,(MATCH(E$1,Petroleum!$C$1:$E$1,0))))/INDEX(Petroleum!$C$25:$E$25,MATCH(E$1,Petroleum!$C$1:$E$1,0))</f>
+        <v>0.43497623825544579</v>
+      </c>
+      <c r="F10" s="20">
+        <f>SUM(INDEX(Petroleum!$C$21:$E$22,0,(MATCH(F$1,Petroleum!$C$1:$E$1,0))))/INDEX(Petroleum!$C$25:$E$25,MATCH(F$1,Petroleum!$C$1:$E$1,0))</f>
+        <v>0.4398607132038862</v>
+      </c>
+      <c r="G10" s="20">
+        <f>SUM(INDEX(Petroleum!$C$21:$E$22,0,(MATCH(G$1,Petroleum!$C$1:$E$1,0))))/INDEX(Petroleum!$C$25:$E$25,MATCH(G$1,Petroleum!$C$1:$E$1,0))</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="H10" s="4">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="I10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="J10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="K10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="L10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="M10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="N10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="O10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="P10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="Q10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="R10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="S10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="T10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="U10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="V10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="W10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="X10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="Y10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="Z10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AA10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AB10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AC10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AD10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AE10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AF10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AG10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AH10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AI10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AJ10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
+      </c>
+      <c r="AK10" s="20">
+        <f>$G10</f>
+        <v>0.43178419220621062</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="17">
-        <v>0</v>
-      </c>
-      <c r="C11" s="17">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <v>0</v>
-      </c>
-      <c r="AI11">
-        <v>0</v>
-      </c>
-      <c r="AJ11">
-        <v>0</v>
-      </c>
-      <c r="AK11">
-        <v>0</v>
+      <c r="A11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="20">
+        <f t="shared" ref="B11:B13" si="0">E11</f>
+        <v>0.24362158738715628</v>
+      </c>
+      <c r="C11" s="20">
+        <f t="shared" ref="C11:C13" si="1">E11</f>
+        <v>0.24362158738715628</v>
+      </c>
+      <c r="D11" s="20">
+        <f t="shared" ref="D11:D12" si="2">E11</f>
+        <v>0.24362158738715628</v>
+      </c>
+      <c r="E11" s="20">
+        <f>SUM(INDEX(Petroleum!$C$12:$E$13,0,(MATCH(E$1,Petroleum!$C$1:$E$1,0))))/INDEX(Petroleum!$C$16:$E$16,MATCH(E$1,Petroleum!$C$1:$E$1,0))</f>
+        <v>0.24362158738715628</v>
+      </c>
+      <c r="F11" s="20">
+        <f>SUM(INDEX(Petroleum!$C$12:$E$13,0,(MATCH(F$1,Petroleum!$C$1:$E$1,0))))/INDEX(Petroleum!$C$16:$E$16,MATCH(F$1,Petroleum!$C$1:$E$1,0))</f>
+        <v>0.23177118348071471</v>
+      </c>
+      <c r="G11" s="20">
+        <f>SUM(INDEX(Petroleum!$C$12:$E$13,0,(MATCH(G$1,Petroleum!$C$1:$E$1,0))))/INDEX(Petroleum!$C$16:$E$16,MATCH(G$1,Petroleum!$C$1:$E$1,0))</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="H11" s="20">
+        <f t="shared" ref="H11:H13" si="3">$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="I11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="J11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="K11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="L11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="M11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="N11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="O11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="P11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="Q11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="R11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="S11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="T11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="U11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="V11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="W11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="X11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="Y11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="Z11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AA11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AB11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AC11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AD11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AE11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AF11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AG11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AH11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AI11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AJ11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AK11" s="20">
+        <f>$G11</f>
+        <v>0.22645117285872568</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="17">
-        <v>0</v>
-      </c>
-      <c r="C12" s="17">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
-      <c r="Z12">
-        <v>0</v>
-      </c>
-      <c r="AA12">
-        <v>0</v>
-      </c>
-      <c r="AB12">
-        <v>0</v>
-      </c>
-      <c r="AC12">
-        <v>0</v>
-      </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
-      <c r="AE12">
-        <v>0</v>
-      </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
-      <c r="AG12">
-        <v>0</v>
-      </c>
-      <c r="AH12">
-        <v>0</v>
-      </c>
-      <c r="AI12">
-        <v>0</v>
-      </c>
-      <c r="AJ12">
-        <v>0</v>
-      </c>
-      <c r="AK12">
-        <v>0</v>
+      <c r="A12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="20">
+        <f t="shared" si="0"/>
+        <v>0.24271674094653878</v>
+      </c>
+      <c r="C12" s="20">
+        <f t="shared" si="1"/>
+        <v>0.24271674094653878</v>
+      </c>
+      <c r="D12" s="20">
+        <f t="shared" si="2"/>
+        <v>0.24271674094653878</v>
+      </c>
+      <c r="E12" s="20">
+        <f>E10*0.558</f>
+        <v>0.24271674094653878</v>
+      </c>
+      <c r="F12" s="20">
+        <f>F10*0.558</f>
+        <v>0.24544227796776852</v>
+      </c>
+      <c r="G12" s="20">
+        <f>G10*0.558</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="H12" s="20">
+        <f t="shared" si="3"/>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="I12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="J12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="K12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="L12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="M12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="N12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="O12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="P12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="Q12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="R12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="S12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="T12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="U12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="V12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="W12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="X12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="Y12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="Z12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AA12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AB12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AC12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AD12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AE12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AF12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AG12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AH12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AI12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AJ12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
+      </c>
+      <c r="AK12" s="20">
+        <f>$G12</f>
+        <v>0.24093557925106554</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="17">
-        <v>0</v>
-      </c>
-      <c r="C13" s="17">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
-      <c r="AB13">
-        <v>0</v>
-      </c>
-      <c r="AC13">
-        <v>0</v>
-      </c>
-      <c r="AD13">
-        <v>0</v>
-      </c>
-      <c r="AE13">
-        <v>0</v>
-      </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
-      <c r="AG13">
-        <v>0</v>
-      </c>
-      <c r="AH13">
-        <v>0</v>
-      </c>
-      <c r="AI13">
-        <v>0</v>
-      </c>
-      <c r="AJ13">
-        <v>0</v>
-      </c>
-      <c r="AK13">
-        <v>0</v>
+      <c r="A13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="20">
+        <f t="shared" si="0"/>
+        <v>0.24362158738715628</v>
+      </c>
+      <c r="C13" s="20">
+        <f t="shared" si="1"/>
+        <v>0.24362158738715628</v>
+      </c>
+      <c r="D13" s="20">
+        <f>E13</f>
+        <v>0.24362158738715628</v>
+      </c>
+      <c r="E13" s="20">
+        <f t="shared" ref="E13:G13" si="4">E11</f>
+        <v>0.24362158738715628</v>
+      </c>
+      <c r="F13" s="20">
+        <f>F11</f>
+        <v>0.23177118348071471</v>
+      </c>
+      <c r="G13" s="20">
+        <f t="shared" si="4"/>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="H13" s="20">
+        <f t="shared" si="3"/>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="I13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="J13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="K13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="L13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="M13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="N13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="O13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="P13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="Q13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="R13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="S13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="T13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="U13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="V13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="W13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="X13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="Y13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="Z13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AA13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AB13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AC13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AD13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AE13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AF13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AG13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AH13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AI13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AJ13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
+      </c>
+      <c r="AK13" s="20">
+        <f>$G13</f>
+        <v>0.22645117285872568</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
+      <c r="A14" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="B14" s="49">
         <f>About!$C$33</f>
@@ -34450,753 +35195,645 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A15" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="20">
-        <f>E15</f>
-        <v>0.43497623825544579</v>
-      </c>
-      <c r="C15" s="20">
-        <f>E15</f>
-        <v>0.43497623825544579</v>
-      </c>
-      <c r="D15" s="4">
-        <f>E15</f>
-        <v>0.43497623825544579</v>
-      </c>
-      <c r="E15" s="20">
-        <f>SUM(INDEX(Petroleum!$C$21:$E$22,0,(MATCH(E$6,Petroleum!$C$1:$E$1,0))))/INDEX(Petroleum!$C$25:$E$25,MATCH(E$6,Petroleum!$C$1:$E$1,0))</f>
-        <v>0.43497623825544579</v>
-      </c>
-      <c r="F15" s="20">
-        <f>SUM(INDEX(Petroleum!$C$21:$E$22,0,(MATCH(F$6,Petroleum!$C$1:$E$1,0))))/INDEX(Petroleum!$C$25:$E$25,MATCH(F$6,Petroleum!$C$1:$E$1,0))</f>
-        <v>0.4398607132038862</v>
-      </c>
-      <c r="G15" s="20">
-        <f>SUM(INDEX(Petroleum!$C$21:$E$22,0,(MATCH(G$6,Petroleum!$C$1:$E$1,0))))/(INDEX(Petroleum!$C$25:$E$25,MATCH(G$6,Petroleum!$C$1:$E$1,0))-SUM(INDEX(Petroleum!$C$21:$E$22,0,(MATCH(G$6,Petroleum!$C$1:$E$1,0)))))</f>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="H15" s="4">
-        <f>$G15</f>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="I15" s="20">
-        <f t="shared" ref="I15:AK18" si="0">$G15</f>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="J15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="K15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="L15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="M15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="N15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="O15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="P15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="Q15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="R15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="S15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="T15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="U15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="V15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="W15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="X15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="Y15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="Z15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AA15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AB15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AC15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AD15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AE15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AF15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AG15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AH15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AI15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AJ15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
-      </c>
-      <c r="AK15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7598947200759838</v>
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="C15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="D15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="E15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="F15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="G15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="H15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="I15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="J15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="K15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="L15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="M15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="N15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="O15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="P15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Q15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="R15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="S15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="T15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="U15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="V15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="W15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="X15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Y15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Z15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AA15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AB15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AC15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AD15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AE15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AF15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AG15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AH15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AI15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AJ15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AK15" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A16" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="20">
-        <f t="shared" ref="B16:B18" si="1">E16</f>
-        <v>0.24362158738715628</v>
-      </c>
-      <c r="C16" s="20">
-        <f t="shared" ref="C16:C18" si="2">E16</f>
-        <v>0.24362158738715628</v>
-      </c>
-      <c r="D16" s="20">
-        <f t="shared" ref="D16:D17" si="3">E16</f>
-        <v>0.24362158738715628</v>
-      </c>
-      <c r="E16" s="20">
-        <f>SUM(INDEX(Petroleum!$C$12:$E$13,0,(MATCH(E$6,Petroleum!$C$1:$E$1,0))))/INDEX(Petroleum!$C$16:$E$16,MATCH(E$6,Petroleum!$C$1:$E$1,0))</f>
-        <v>0.24362158738715628</v>
-      </c>
-      <c r="F16" s="20">
-        <f>SUM(INDEX(Petroleum!$C$12:$E$13,0,(MATCH(F$6,Petroleum!$C$1:$E$1,0))))/INDEX(Petroleum!$C$16:$E$16,MATCH(F$6,Petroleum!$C$1:$E$1,0))</f>
-        <v>0.23177118348071471</v>
-      </c>
-      <c r="G16" s="20">
-        <f>SUM(INDEX(Petroleum!$C$12:$E$13,0,(MATCH(G$6,Petroleum!$C$1:$E$1,0))))/(INDEX(Petroleum!$C$16:$E$16,MATCH(G$6,Petroleum!$C$1:$E$1,0))-SUM(INDEX(Petroleum!$C$12:$E$13,0,(MATCH(G$6,Petroleum!$C$1:$E$1,0)))))</f>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="H16" s="20">
-        <f t="shared" ref="H16:H18" si="4">$G16</f>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="I16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="J16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="K16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="L16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="M16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="N16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="O16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="P16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="Q16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="R16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="S16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="T16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="U16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="V16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="W16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="X16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="Y16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="Z16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AA16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AB16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AC16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AD16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AE16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AF16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AG16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AH16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AI16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AJ16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AK16" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="17">
+        <v>0</v>
+      </c>
+      <c r="C16" s="17">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+      <c r="AJ16">
+        <v>0</v>
+      </c>
+      <c r="AK16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A17" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="20">
-        <f t="shared" si="1"/>
-        <v>0.24271674094653878</v>
-      </c>
-      <c r="C17" s="20">
-        <f t="shared" si="2"/>
-        <v>0.24271674094653878</v>
-      </c>
-      <c r="D17" s="20">
-        <f t="shared" si="3"/>
-        <v>0.24271674094653878</v>
-      </c>
-      <c r="E17" s="20">
-        <f t="shared" ref="E17:G17" si="5">E15*0.558</f>
-        <v>0.24271674094653878</v>
-      </c>
-      <c r="F17" s="20">
-        <f>F15*0.558</f>
-        <v>0.24544227796776852</v>
-      </c>
-      <c r="G17" s="20">
-        <f t="shared" si="5"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="H17" s="20">
-        <f t="shared" si="4"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="I17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="J17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="K17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="L17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="M17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="N17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="O17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="P17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="Q17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="R17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="S17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="T17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="U17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="V17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="W17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="X17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="Y17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="Z17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AA17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AB17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AC17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AD17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AE17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AF17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AG17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AH17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AI17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AJ17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
-      </c>
-      <c r="AK17" s="20">
-        <f t="shared" si="0"/>
-        <v>0.42402125380239902</v>
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="C17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="D17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="E17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="F17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="G17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="H17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="I17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="J17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="K17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="L17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="M17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="N17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="O17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="P17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Q17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="R17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="S17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="T17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="U17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="V17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="W17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="X17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Y17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Z17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AA17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AB17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AC17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AD17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AE17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AF17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AG17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AH17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AI17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AJ17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AK17" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A18" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="20">
-        <f t="shared" si="1"/>
-        <v>0.24362158738715628</v>
-      </c>
-      <c r="C18" s="20">
-        <f t="shared" si="2"/>
-        <v>0.24362158738715628</v>
-      </c>
-      <c r="D18" s="20">
-        <f>E18</f>
-        <v>0.24362158738715628</v>
-      </c>
-      <c r="E18" s="20">
-        <f t="shared" ref="E18:G18" si="6">E16</f>
-        <v>0.24362158738715628</v>
-      </c>
-      <c r="F18" s="20">
-        <f>F16</f>
-        <v>0.23177118348071471</v>
-      </c>
-      <c r="G18" s="20">
-        <f t="shared" si="6"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="H18" s="20">
-        <f t="shared" si="4"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="I18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="J18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="K18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="L18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="M18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="N18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="O18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="P18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="Q18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="R18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="S18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="T18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="U18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="V18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="W18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="X18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="Y18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="Z18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AA18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AB18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AC18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AD18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AE18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AF18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AG18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AH18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AI18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AJ18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
-      </c>
-      <c r="AK18" s="20">
-        <f t="shared" si="0"/>
-        <v>0.29274321789821367</v>
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="17">
+        <v>0</v>
+      </c>
+      <c r="C18" s="17">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A19" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="C19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="D19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="E19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="F19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="G19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="H19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="I19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="J19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="K19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="L19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="M19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="N19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="O19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="P19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Q19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="R19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="S19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="T19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="U19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="V19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="W19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="X19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Y19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Z19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AA19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AB19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AC19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AD19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AE19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AF19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AG19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AH19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AI19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AJ19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AK19" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="17">
+        <v>0</v>
+      </c>
+      <c r="C19" s="17">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <v>0</v>
+      </c>
+      <c r="AJ19">
+        <v>0</v>
+      </c>
+      <c r="AK19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B20" s="49">
         <f>About!$C$33</f>
@@ -35345,120 +35982,156 @@
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="17">
-        <v>0</v>
-      </c>
-      <c r="C21" s="17">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21">
-        <v>0</v>
-      </c>
-      <c r="Z21">
-        <v>0</v>
-      </c>
-      <c r="AA21">
-        <v>0</v>
-      </c>
-      <c r="AB21">
-        <v>0</v>
-      </c>
-      <c r="AC21">
-        <v>0</v>
-      </c>
-      <c r="AD21">
-        <v>0</v>
-      </c>
-      <c r="AE21">
-        <v>0</v>
-      </c>
-      <c r="AF21">
-        <v>0</v>
-      </c>
-      <c r="AG21">
-        <v>0</v>
-      </c>
-      <c r="AH21">
-        <v>0</v>
-      </c>
-      <c r="AI21">
-        <v>0</v>
-      </c>
-      <c r="AJ21">
-        <v>0</v>
-      </c>
-      <c r="AK21">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="B21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="C21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="D21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="E21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="F21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="G21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="H21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="I21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="J21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="K21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="L21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="M21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="N21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="O21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="P21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Q21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="R21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="S21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="T21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="U21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="V21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="W21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="X21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Y21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="Z21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AA21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AB21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AC21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AD21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AE21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AF21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AG21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AH21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AI21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AJ21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
+      </c>
+      <c r="AK21" s="49">
+        <f>About!$C$33</f>
+        <v>1.4633182249393908E-2</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B22" s="49">
         <f>About!$C$33</f>
@@ -35601,679 +36274,6 @@
         <v>1.4633182249393908E-2</v>
       </c>
       <c r="AK22" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="17">
-        <v>0</v>
-      </c>
-      <c r="C23" s="17">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
-      <c r="V23">
-        <v>0</v>
-      </c>
-      <c r="W23">
-        <v>0</v>
-      </c>
-      <c r="X23">
-        <v>0</v>
-      </c>
-      <c r="Y23">
-        <v>0</v>
-      </c>
-      <c r="Z23">
-        <v>0</v>
-      </c>
-      <c r="AA23">
-        <v>0</v>
-      </c>
-      <c r="AB23">
-        <v>0</v>
-      </c>
-      <c r="AC23">
-        <v>0</v>
-      </c>
-      <c r="AD23">
-        <v>0</v>
-      </c>
-      <c r="AE23">
-        <v>0</v>
-      </c>
-      <c r="AF23">
-        <v>0</v>
-      </c>
-      <c r="AG23">
-        <v>0</v>
-      </c>
-      <c r="AH23">
-        <v>0</v>
-      </c>
-      <c r="AI23">
-        <v>0</v>
-      </c>
-      <c r="AJ23">
-        <v>0</v>
-      </c>
-      <c r="AK23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="17">
-        <v>0</v>
-      </c>
-      <c r="C24" s="17">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
-      <c r="V24">
-        <v>0</v>
-      </c>
-      <c r="W24">
-        <v>0</v>
-      </c>
-      <c r="X24">
-        <v>0</v>
-      </c>
-      <c r="Y24">
-        <v>0</v>
-      </c>
-      <c r="Z24">
-        <v>0</v>
-      </c>
-      <c r="AA24">
-        <v>0</v>
-      </c>
-      <c r="AB24">
-        <v>0</v>
-      </c>
-      <c r="AC24">
-        <v>0</v>
-      </c>
-      <c r="AD24">
-        <v>0</v>
-      </c>
-      <c r="AE24">
-        <v>0</v>
-      </c>
-      <c r="AF24">
-        <v>0</v>
-      </c>
-      <c r="AG24">
-        <v>0</v>
-      </c>
-      <c r="AH24">
-        <v>0</v>
-      </c>
-      <c r="AI24">
-        <v>0</v>
-      </c>
-      <c r="AJ24">
-        <v>0</v>
-      </c>
-      <c r="AK24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="C25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="D25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="E25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="F25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="G25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="H25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="I25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="J25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="K25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="L25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="M25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="N25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="O25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="P25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Q25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="R25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="S25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="T25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="U25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="V25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="W25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="X25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Y25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Z25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AA25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AB25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AC25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AD25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AE25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AF25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AG25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AH25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AI25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AJ25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AK25" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="C26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="D26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="E26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="F26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="G26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="H26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="I26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="J26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="K26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="L26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="M26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="N26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="O26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="P26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Q26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="R26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="S26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="T26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="U26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="V26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="W26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="X26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Y26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Z26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AA26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AB26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AC26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AD26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AE26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AF26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AG26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AH26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AI26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AJ26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AK26" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="C27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="D27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="E27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="F27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="G27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="H27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="I27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="J27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="K27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="L27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="M27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="N27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="O27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="P27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Q27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="R27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="S27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="T27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="U27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="V27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="W27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="X27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Y27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="Z27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AA27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AB27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AC27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AD27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AE27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AF27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AG27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AH27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AI27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AJ27" s="49">
-        <f>About!$C$33</f>
-        <v>1.4633182249393908E-2</v>
-      </c>
-      <c r="AK27" s="49">
         <f>About!$C$33</f>
         <v>1.4633182249393908E-2</v>
       </c>

</xml_diff>